<commit_message>
adding RNA sample and library files for January ZEV experiments
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97723C9-CB2A-7E4D-8BB9-FF1DC68527D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20280" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -76,29 +85,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,63 +121,68 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -352,20 +372,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="5" max="6" width="7" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +447,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -425,7 +455,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>14</v>
@@ -439,16 +469,16 @@
         <v>16</v>
       </c>
       <c r="I2" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L2" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -465,7 +495,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -473,7 +503,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
@@ -487,16 +517,16 @@
         <v>16</v>
       </c>
       <c r="I3" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K3" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L3" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -513,7 +543,7 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -521,7 +551,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -535,16 +565,16 @@
         <v>16</v>
       </c>
       <c r="I4" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L4" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -561,7 +591,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -569,7 +599,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
@@ -583,16 +613,16 @@
         <v>16</v>
       </c>
       <c r="I5" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K5" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L5" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -609,7 +639,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -617,7 +647,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>14</v>
@@ -631,16 +661,16 @@
         <v>16</v>
       </c>
       <c r="I6" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L6" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -657,7 +687,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -665,7 +695,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
@@ -679,16 +709,16 @@
         <v>16</v>
       </c>
       <c r="I7" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L7" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -705,7 +735,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -713,7 +743,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
@@ -727,16 +757,16 @@
         <v>16</v>
       </c>
       <c r="I8" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L8" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -753,7 +783,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -761,7 +791,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
@@ -775,16 +805,16 @@
         <v>16</v>
       </c>
       <c r="I9" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L9" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -801,7 +831,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -809,7 +839,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>14</v>
@@ -823,16 +853,16 @@
         <v>16</v>
       </c>
       <c r="I10" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L10" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -849,7 +879,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -857,7 +887,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>14</v>
@@ -871,16 +901,16 @@
         <v>16</v>
       </c>
       <c r="I11" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K11" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L11" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -897,7 +927,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -905,7 +935,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>14</v>
@@ -919,16 +949,16 @@
         <v>16</v>
       </c>
       <c r="I12" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L12" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -945,7 +975,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>14</v>
@@ -967,16 +997,16 @@
         <v>16</v>
       </c>
       <c r="I13" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L13" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -993,7 +1023,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1001,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>14</v>
@@ -1015,16 +1045,16 @@
         <v>16</v>
       </c>
       <c r="I14" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L14" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1041,7 +1071,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1049,7 +1079,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="9">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>14</v>
@@ -1063,16 +1093,16 @@
         <v>16</v>
       </c>
       <c r="I15" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K15" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L15" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1089,7 +1119,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1127,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="9">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>14</v>
@@ -1111,16 +1141,16 @@
         <v>16</v>
       </c>
       <c r="I16" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K16" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L16" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1137,7 +1167,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1145,7 +1175,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>14</v>
@@ -1159,16 +1189,16 @@
         <v>16</v>
       </c>
       <c r="I17" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K17" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L17" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1185,7 +1215,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1223,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>14</v>
@@ -1207,16 +1237,16 @@
         <v>16</v>
       </c>
       <c r="I18" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L18" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1233,7 +1263,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1241,7 +1271,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="9">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>14</v>
@@ -1255,16 +1285,16 @@
         <v>16</v>
       </c>
       <c r="I19" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K19" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L19" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1281,7 +1311,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1289,7 +1319,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="9">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>14</v>
@@ -1303,16 +1333,16 @@
         <v>16</v>
       </c>
       <c r="I20" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K20" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L20" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1329,7 +1359,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1337,7 +1367,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>14</v>
@@ -1351,16 +1381,16 @@
         <v>16</v>
       </c>
       <c r="I21" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K21" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L21" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1377,7 +1407,7 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1385,7 +1415,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>14</v>
@@ -1399,16 +1429,16 @@
         <v>16</v>
       </c>
       <c r="I22" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K22" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L22" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1425,7 +1455,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -1433,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="9">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>14</v>
@@ -1447,16 +1477,16 @@
         <v>16</v>
       </c>
       <c r="I23" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K23" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L23" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1473,7 +1503,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1481,7 +1511,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="9">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>14</v>
@@ -1495,16 +1525,16 @@
         <v>16</v>
       </c>
       <c r="I24" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L24" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1521,7 +1551,7 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1529,7 +1559,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>14</v>
@@ -1543,16 +1573,16 @@
         <v>16</v>
       </c>
       <c r="I25" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K25" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L25" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1569,7 +1599,7 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1577,7 +1607,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>14</v>
@@ -1591,16 +1621,16 @@
         <v>16</v>
       </c>
       <c r="I26" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L26" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1617,7 +1647,7 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1625,7 +1655,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="9">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>14</v>
@@ -1639,16 +1669,16 @@
         <v>16</v>
       </c>
       <c r="I27" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K27" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L27" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1665,7 +1695,7 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1673,7 +1703,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="9">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>14</v>
@@ -1687,16 +1717,16 @@
         <v>16</v>
       </c>
       <c r="I28" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K28" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L28" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1713,7 +1743,7 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1751,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>14</v>
@@ -1735,16 +1765,16 @@
         <v>16</v>
       </c>
       <c r="I29" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K29" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L29" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1761,7 +1791,7 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1769,7 +1799,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>14</v>
@@ -1783,16 +1813,16 @@
         <v>16</v>
       </c>
       <c r="I30" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L30" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1809,7 +1839,7 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1817,7 +1847,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="9">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>14</v>
@@ -1831,16 +1861,16 @@
         <v>16</v>
       </c>
       <c r="I31" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K31" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L31" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1857,7 +1887,7 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
@@ -1865,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="9">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>14</v>
@@ -1879,16 +1909,16 @@
         <v>16</v>
       </c>
       <c r="I32" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K32" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L32" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1905,7 +1935,7 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
@@ -1913,7 +1943,7 @@
         <v>13</v>
       </c>
       <c r="C33" s="3">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>14</v>
@@ -1927,16 +1957,16 @@
         <v>16</v>
       </c>
       <c r="I33" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K33" s="7">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="L33" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -1953,7 +1983,7 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1961,7 +1991,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="3">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>14</v>
@@ -1975,16 +2005,16 @@
         <v>16</v>
       </c>
       <c r="I34" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L34" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2001,7 +2031,7 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
@@ -2009,7 +2039,7 @@
         <v>13</v>
       </c>
       <c r="C35" s="9">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>14</v>
@@ -2023,16 +2053,16 @@
         <v>16</v>
       </c>
       <c r="I35" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K35" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L35" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -2049,7 +2079,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -2057,7 +2087,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="9">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>14</v>
@@ -2071,16 +2101,16 @@
         <v>16</v>
       </c>
       <c r="I36" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L36" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2097,7 +2127,7 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
@@ -2105,7 +2135,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="3">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>14</v>
@@ -2119,16 +2149,16 @@
         <v>16</v>
       </c>
       <c r="I37" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K37" s="7">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="L37" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -2145,7 +2175,7 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -2153,7 +2183,7 @@
         <v>13</v>
       </c>
       <c r="C38" s="3">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>14</v>
@@ -2167,16 +2197,16 @@
         <v>16</v>
       </c>
       <c r="I38" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K38" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L38" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -2193,7 +2223,7 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -2201,7 +2231,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="9">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>14</v>
@@ -2215,16 +2245,16 @@
         <v>16</v>
       </c>
       <c r="I39" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K39" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="L39" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -2241,7 +2271,7 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
@@ -2249,7 +2279,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="9">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>14</v>
@@ -2263,16 +2293,16 @@
         <v>16</v>
       </c>
       <c r="I40" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K40" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L40" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -2289,7 +2319,7 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -2297,7 +2327,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>14</v>
@@ -2311,16 +2341,16 @@
         <v>16</v>
       </c>
       <c r="I41" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K41" s="7">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="L41" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -2338,6 +2368,6 @@
       <c r="Z41" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
further cleaning to metadata
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
@@ -1,119 +1,149 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97723C9-CB2A-7E4D-8BB9-FF1DC68527D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20280" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="20">
   <si>
-    <t>harvestDate</t>
+    <t xml:space="preserve">harvestDate</t>
   </si>
   <si>
-    <t>harvester</t>
+    <t xml:space="preserve">harvester</t>
   </si>
   <si>
-    <t>biosampleNumber</t>
+    <t xml:space="preserve">biosampleNumber</t>
   </si>
   <si>
-    <t>experimentDesign</t>
+    <t xml:space="preserve">experimentDesign</t>
   </si>
   <si>
-    <t>experimentObservations</t>
+    <t xml:space="preserve">experimentObservations</t>
   </si>
   <si>
-    <t>strain</t>
+    <t xml:space="preserve">strain</t>
   </si>
   <si>
-    <t>genotype</t>
+    <t xml:space="preserve">genotype</t>
   </si>
   <si>
-    <t>floodmedia</t>
+    <t xml:space="preserve">floodmedia</t>
   </si>
   <si>
-    <t>inductionDelay</t>
+    <t xml:space="preserve">inductionDelay</t>
   </si>
   <si>
-    <t>treatment</t>
+    <t xml:space="preserve">treatment</t>
   </si>
   <si>
-    <t>timePoint</t>
+    <t xml:space="preserve">timePoint</t>
   </si>
   <si>
-    <t>replicate</t>
+    <t xml:space="preserve">replicate</t>
   </si>
   <si>
-    <t>01.07.20</t>
+    <t xml:space="preserve">01.07.20</t>
   </si>
   <si>
-    <t>J.PLAGGENBERG</t>
+    <t xml:space="preserve">J.PLAGGENBERG</t>
   </si>
   <si>
-    <t>ZEV_induction</t>
+    <t xml:space="preserve">ZEV_induction</t>
   </si>
   <si>
-    <t>CST6</t>
+    <t xml:space="preserve">CST6</t>
   </si>
   <si>
-    <t>SCGal</t>
+    <t xml:space="preserve">SCGal</t>
   </si>
   <si>
-    <t>EtoH</t>
+    <t xml:space="preserve">EtOH</t>
   </si>
   <si>
-    <t>Estradiol</t>
+    <t xml:space="preserve">Estradiol</t>
   </si>
   <si>
-    <t>RGM1</t>
+    <t xml:space="preserve">RGM1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,15 +154,8 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
+  <borders count="1">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -140,262 +163,107 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
-  <a:themeElements>
-    <a:clrScheme name="Sheets">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4285F4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="EA4335"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="FBBC04"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="34A853"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="FF6D01"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="46BDC6"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="1155CC"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="1155CC"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Sheets">
-      <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="5" max="6" width="7" customWidth="1"/>
-    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,14 +315,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -468,16 +336,16 @@
       <c r="H2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="6">
-        <v>30</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M2" s="1"/>
@@ -495,14 +363,14 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="9" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -516,16 +384,16 @@
       <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="1"/>
@@ -543,14 +411,14 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="9" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -564,16 +432,16 @@
       <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="6">
-        <v>30</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="7">
-        <v>15</v>
-      </c>
-      <c r="L4" s="8">
+      <c r="K4" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M4" s="1"/>
@@ -591,14 +459,14 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -612,16 +480,16 @@
       <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="7">
-        <v>15</v>
-      </c>
-      <c r="L5" s="8">
+      <c r="K5" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L5" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M5" s="1"/>
@@ -639,14 +507,14 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -660,16 +528,16 @@
       <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="6">
-        <v>30</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M6" s="1"/>
@@ -687,14 +555,14 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="9" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -708,16 +576,16 @@
       <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M7" s="1"/>
@@ -735,14 +603,14 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="9" t="n">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -756,16 +624,16 @@
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="6">
-        <v>30</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="6">
-        <v>30</v>
-      </c>
-      <c r="L8" s="8">
+      <c r="K8" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L8" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M8" s="1"/>
@@ -783,14 +651,14 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -804,16 +672,16 @@
       <c r="H9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="6">
-        <v>30</v>
-      </c>
-      <c r="L9" s="8">
+      <c r="K9" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L9" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M9" s="1"/>
@@ -831,14 +699,14 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="3" t="n">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -852,16 +720,16 @@
       <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="6">
-        <v>30</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I10" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="9" t="n">
         <v>3</v>
       </c>
       <c r="M10" s="1"/>
@@ -879,14 +747,14 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="9" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -900,16 +768,16 @@
       <c r="H11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="9" t="n">
         <v>3</v>
       </c>
       <c r="M11" s="1"/>
@@ -927,14 +795,14 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="9" t="n">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -948,16 +816,16 @@
       <c r="H12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="6">
-        <v>30</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="I12" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M12" s="1"/>
@@ -975,14 +843,14 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -996,16 +864,16 @@
       <c r="H13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M13" s="1"/>
@@ -1023,14 +891,14 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="3" t="n">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1044,16 +912,16 @@
       <c r="H14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="6">
-        <v>30</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I14" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="7">
-        <v>15</v>
-      </c>
-      <c r="L14" s="8">
+      <c r="K14" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L14" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M14" s="1"/>
@@ -1071,14 +939,14 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="9" t="n">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1092,16 +960,16 @@
       <c r="H15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="7">
-        <v>15</v>
-      </c>
-      <c r="L15" s="8">
+      <c r="K15" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L15" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M15" s="1"/>
@@ -1119,14 +987,14 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="9" t="n">
         <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1140,16 +1008,16 @@
       <c r="H16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="6">
-        <v>30</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="I16" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M16" s="1"/>
@@ -1167,14 +1035,14 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="3" t="n">
         <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1188,16 +1056,16 @@
       <c r="H17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M17" s="1"/>
@@ -1215,14 +1083,14 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="3" t="n">
         <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -1236,16 +1104,16 @@
       <c r="H18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="6">
-        <v>30</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="I18" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="6">
-        <v>30</v>
-      </c>
-      <c r="L18" s="8">
+      <c r="K18" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L18" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M18" s="1"/>
@@ -1263,14 +1131,14 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="9" t="n">
         <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1284,16 +1152,16 @@
       <c r="H19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="6">
-        <v>30</v>
-      </c>
-      <c r="L19" s="8">
+      <c r="K19" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L19" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M19" s="1"/>
@@ -1311,14 +1179,14 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="9" t="n">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -1332,16 +1200,16 @@
       <c r="H20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="6">
-        <v>30</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="I20" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="9" t="n">
         <v>4</v>
       </c>
       <c r="M20" s="1"/>
@@ -1359,14 +1227,14 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="3" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -1380,16 +1248,16 @@
       <c r="H21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="9" t="n">
         <v>4</v>
       </c>
       <c r="M21" s="1"/>
@@ -1407,14 +1275,14 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="3" t="n">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -1428,16 +1296,16 @@
       <c r="H22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="6">
-        <v>30</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="I22" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L22" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M22" s="1"/>
@@ -1455,14 +1323,14 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="9" t="n">
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -1476,16 +1344,16 @@
       <c r="H23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L23" s="8">
+      <c r="L23" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M23" s="1"/>
@@ -1503,14 +1371,14 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="9" t="n">
         <v>23</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -1524,16 +1392,16 @@
       <c r="H24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="6">
-        <v>30</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="I24" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="7">
-        <v>15</v>
-      </c>
-      <c r="L24" s="8">
+      <c r="K24" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L24" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M24" s="1"/>
@@ -1551,14 +1419,14 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="3" t="n">
         <v>24</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -1572,16 +1440,16 @@
       <c r="H25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="7">
-        <v>15</v>
-      </c>
-      <c r="L25" s="8">
+      <c r="K25" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L25" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M25" s="1"/>
@@ -1599,14 +1467,14 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="3" t="n">
         <v>25</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -1620,16 +1488,16 @@
       <c r="H26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="6">
-        <v>30</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="I26" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M26" s="1"/>
@@ -1647,14 +1515,14 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="9" t="n">
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -1668,16 +1536,16 @@
       <c r="H27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L27" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M27" s="1"/>
@@ -1695,14 +1563,14 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="9" t="n">
         <v>27</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -1716,16 +1584,16 @@
       <c r="H28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="6">
-        <v>30</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="I28" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="6">
-        <v>30</v>
-      </c>
-      <c r="L28" s="8">
+      <c r="K28" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L28" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M28" s="1"/>
@@ -1743,14 +1611,14 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="3" t="n">
         <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -1764,16 +1632,16 @@
       <c r="H29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="6">
-        <v>30</v>
-      </c>
-      <c r="L29" s="8">
+      <c r="K29" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L29" s="8" t="n">
         <v>3</v>
       </c>
       <c r="M29" s="1"/>
@@ -1791,14 +1659,14 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="3" t="n">
         <v>29</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -1812,16 +1680,16 @@
       <c r="H30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="6">
-        <v>30</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="I30" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="9" t="n">
         <v>3</v>
       </c>
       <c r="M30" s="1"/>
@@ -1839,14 +1707,14 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="9" t="n">
         <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -1860,16 +1728,16 @@
       <c r="H31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="9" t="n">
         <v>3</v>
       </c>
       <c r="M31" s="1"/>
@@ -1887,14 +1755,14 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="9" t="n">
         <v>31</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -1908,16 +1776,16 @@
       <c r="H32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="6">
-        <v>30</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="I32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J32" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L32" s="8">
+      <c r="L32" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M32" s="1"/>
@@ -1935,14 +1803,14 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="3" t="n">
         <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -1956,16 +1824,16 @@
       <c r="H33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="8" t="n">
         <v>-1</v>
       </c>
-      <c r="L33" s="8">
+      <c r="L33" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M33" s="1"/>
@@ -1983,14 +1851,14 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="3" t="n">
         <v>33</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -2004,16 +1872,16 @@
       <c r="H34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="6">
-        <v>30</v>
-      </c>
-      <c r="J34" s="1" t="s">
+      <c r="I34" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="7">
-        <v>15</v>
-      </c>
-      <c r="L34" s="8">
+      <c r="K34" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L34" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M34" s="1"/>
@@ -2031,14 +1899,14 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="9" t="n">
         <v>34</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -2052,16 +1920,16 @@
       <c r="H35" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="7">
-        <v>15</v>
-      </c>
-      <c r="L35" s="8">
+      <c r="K35" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="L35" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M35" s="1"/>
@@ -2079,14 +1947,14 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="9" t="n">
         <v>35</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -2100,16 +1968,16 @@
       <c r="H36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="6">
-        <v>30</v>
-      </c>
-      <c r="J36" s="1" t="s">
+      <c r="I36" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K36" s="7">
+      <c r="K36" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L36" s="8">
+      <c r="L36" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M36" s="1"/>
@@ -2127,14 +1995,14 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="3" t="n">
         <v>36</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -2148,16 +2016,16 @@
       <c r="H37" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K37" s="7">
+      <c r="K37" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="L37" s="8">
+      <c r="L37" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M37" s="1"/>
@@ -2175,14 +2043,14 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="3" t="n">
         <v>37</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -2196,16 +2064,16 @@
       <c r="H38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="6">
-        <v>30</v>
-      </c>
-      <c r="J38" s="1" t="s">
+      <c r="I38" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="6">
-        <v>30</v>
-      </c>
-      <c r="L38" s="8">
+      <c r="K38" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L38" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M38" s="1"/>
@@ -2223,14 +2091,14 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="9" t="n">
         <v>38</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -2244,16 +2112,16 @@
       <c r="H39" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K39" s="6">
-        <v>30</v>
-      </c>
-      <c r="L39" s="8">
+      <c r="K39" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="L39" s="8" t="n">
         <v>4</v>
       </c>
       <c r="M39" s="1"/>
@@ -2271,14 +2139,14 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="9" t="n">
         <v>39</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -2292,16 +2160,16 @@
       <c r="H40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="6">
-        <v>30</v>
-      </c>
-      <c r="J40" s="1" t="s">
+      <c r="I40" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J40" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L40" s="9">
+      <c r="L40" s="9" t="n">
         <v>4</v>
       </c>
       <c r="M40" s="1"/>
@@ -2319,14 +2187,14 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="3" t="n">
         <v>40</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -2340,16 +2208,16 @@
       <c r="H41" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="6" t="n">
         <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="8" t="n">
         <v>90</v>
       </c>
-      <c r="L41" s="9">
+      <c r="L41" s="9" t="n">
         <v>4</v>
       </c>
       <c r="M41" s="1"/>
@@ -2368,6 +2236,12 @@
       <c r="Z41" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifying files from the ZEV jan reps that had major inconsistencies
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D44BFB6-B84D-AC44-B774-FEAA0DBEF2DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="13000" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -22,95 +35,76 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="20">
   <si>
-    <t xml:space="preserve">harvestDate</t>
+    <t>harvestDate</t>
   </si>
   <si>
-    <t xml:space="preserve">harvester</t>
+    <t>harvester</t>
   </si>
   <si>
-    <t xml:space="preserve">bioSampleNumber</t>
+    <t>bioSampleNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">experimentDesign</t>
+    <t>experimentDesign</t>
   </si>
   <si>
-    <t xml:space="preserve">experimentObservations</t>
+    <t>experimentObservations</t>
   </si>
   <si>
-    <t xml:space="preserve">strain</t>
+    <t>strain</t>
   </si>
   <si>
-    <t xml:space="preserve">genotype</t>
+    <t>genotype</t>
   </si>
   <si>
-    <t xml:space="preserve">floodmedia</t>
+    <t>floodmedia</t>
   </si>
   <si>
-    <t xml:space="preserve">inductionDelay</t>
+    <t>inductionDelay</t>
   </si>
   <si>
-    <t xml:space="preserve">treatment</t>
+    <t>treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">timePoint</t>
+    <t>timePoint</t>
   </si>
   <si>
-    <t xml:space="preserve">replicate</t>
+    <t>replicate</t>
   </si>
   <si>
-    <t xml:space="preserve">01.07.20</t>
+    <t>01.07.20</t>
   </si>
   <si>
-    <t xml:space="preserve">J.PLAGGENBERG</t>
+    <t>J.PLAGGENBERG</t>
   </si>
   <si>
-    <t xml:space="preserve">ZEV_induction</t>
+    <t>ZEV_induction</t>
   </si>
   <si>
-    <t xml:space="preserve">CST6</t>
+    <t>CST6</t>
   </si>
   <si>
-    <t xml:space="preserve">SCGal</t>
+    <t>SCGal</t>
   </si>
   <si>
-    <t xml:space="preserve">EtOH</t>
+    <t>EtOH</t>
   </si>
   <si>
-    <t xml:space="preserve">Estradiol</t>
+    <t>Estradiol</t>
   </si>
   <si>
-    <t xml:space="preserve">RGM1</t>
+    <t>RGM1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,7 +143,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -162,7 +155,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -170,111 +163,366 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="14.5"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="6" width="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="13" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -326,14 +574,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -347,16 +595,16 @@
       <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="n">
+      <c r="I2" s="7">
         <v>30</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="K2" s="9">
         <v>-1</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="9">
         <v>3</v>
       </c>
       <c r="M2" s="1"/>
@@ -374,14 +622,14 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="10">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -395,16 +643,16 @@
       <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="7" t="n">
+      <c r="I3" s="7">
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="9" t="n">
+      <c r="K3" s="9">
         <v>-1</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="9">
         <v>3</v>
       </c>
       <c r="M3" s="1"/>
@@ -422,14 +670,14 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="10">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -443,16 +691,16 @@
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="7">
         <v>30</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L4" s="9" t="n">
+      <c r="K4" s="9">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9">
         <v>3</v>
       </c>
       <c r="M4" s="1"/>
@@ -470,14 +718,14 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -491,16 +739,16 @@
       <c r="H5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="7">
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L5" s="9" t="n">
+      <c r="K5" s="9">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9">
         <v>3</v>
       </c>
       <c r="M5" s="1"/>
@@ -518,14 +766,14 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -539,16 +787,16 @@
       <c r="H6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="7">
         <v>30</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="9">
         <v>20</v>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="9">
         <v>3</v>
       </c>
       <c r="M6" s="1"/>
@@ -566,14 +814,14 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="10">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -587,16 +835,16 @@
       <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="7">
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="9">
         <v>20</v>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="9">
         <v>3</v>
       </c>
       <c r="M7" s="1"/>
@@ -614,14 +862,14 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="10">
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -635,16 +883,16 @@
       <c r="H8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="7">
         <v>30</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L8" s="9" t="n">
+      <c r="K8" s="7">
+        <v>30</v>
+      </c>
+      <c r="L8" s="9">
         <v>3</v>
       </c>
       <c r="M8" s="1"/>
@@ -662,14 +910,14 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="4">
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -683,16 +931,16 @@
       <c r="H9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="7">
         <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L9" s="9" t="n">
+      <c r="K9" s="7">
+        <v>30</v>
+      </c>
+      <c r="L9" s="9">
         <v>3</v>
       </c>
       <c r="M9" s="1"/>
@@ -710,14 +958,14 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="4">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -731,16 +979,16 @@
       <c r="H10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="7">
         <v>30</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="9" t="n">
+      <c r="K10" s="9">
         <v>90</v>
       </c>
-      <c r="L10" s="10" t="n">
+      <c r="L10" s="10">
         <v>3</v>
       </c>
       <c r="M10" s="1"/>
@@ -758,14 +1006,14 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="10">
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -779,16 +1027,16 @@
       <c r="H11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="7">
         <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="9" t="n">
+      <c r="K11" s="9">
         <v>90</v>
       </c>
-      <c r="L11" s="10" t="n">
+      <c r="L11" s="10">
         <v>3</v>
       </c>
       <c r="M11" s="1"/>
@@ -806,14 +1054,14 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="10">
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -827,16 +1075,16 @@
       <c r="H12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="7">
         <v>30</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="9">
         <v>-1</v>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="9">
         <v>4</v>
       </c>
       <c r="M12" s="1"/>
@@ -854,14 +1102,14 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="4">
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -875,16 +1123,16 @@
       <c r="H13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="7">
         <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="9" t="n">
+      <c r="K13" s="9">
         <v>-1</v>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="9">
         <v>4</v>
       </c>
       <c r="M13" s="1"/>
@@ -902,14 +1150,14 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C14" s="4">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -923,16 +1171,16 @@
       <c r="H14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I14" s="7">
         <v>30</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L14" s="9" t="n">
+      <c r="K14" s="9">
+        <v>15</v>
+      </c>
+      <c r="L14" s="9">
         <v>4</v>
       </c>
       <c r="M14" s="1"/>
@@ -950,14 +1198,14 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="10">
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -971,16 +1219,16 @@
       <c r="H15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="7">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L15" s="9" t="n">
+      <c r="K15" s="9">
+        <v>15</v>
+      </c>
+      <c r="L15" s="9">
         <v>4</v>
       </c>
       <c r="M15" s="1"/>
@@ -998,14 +1246,14 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="10">
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1019,16 +1267,16 @@
       <c r="H16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="7" t="n">
+      <c r="I16" s="7">
         <v>30</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="9" t="n">
+      <c r="K16" s="9">
         <v>20</v>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="L16" s="9">
         <v>4</v>
       </c>
       <c r="M16" s="1"/>
@@ -1046,14 +1294,14 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="C17" s="4">
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -1067,16 +1315,16 @@
       <c r="H17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="7">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="9" t="n">
+      <c r="K17" s="9">
         <v>20</v>
       </c>
-      <c r="L17" s="9" t="n">
+      <c r="L17" s="9">
         <v>4</v>
       </c>
       <c r="M17" s="1"/>
@@ -1094,14 +1342,14 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="C18" s="4">
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1115,16 +1363,16 @@
       <c r="H18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="7">
         <v>30</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L18" s="9" t="n">
+      <c r="K18" s="7">
+        <v>30</v>
+      </c>
+      <c r="L18" s="9">
         <v>4</v>
       </c>
       <c r="M18" s="1"/>
@@ -1142,14 +1390,14 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="10">
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1163,16 +1411,16 @@
       <c r="H19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I19" s="7">
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L19" s="9" t="n">
+      <c r="K19" s="7">
+        <v>30</v>
+      </c>
+      <c r="L19" s="9">
         <v>4</v>
       </c>
       <c r="M19" s="1"/>
@@ -1190,14 +1438,14 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="10">
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1211,16 +1459,16 @@
       <c r="H20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="7">
         <v>30</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="9" t="n">
+      <c r="K20" s="9">
         <v>90</v>
       </c>
-      <c r="L20" s="10" t="n">
+      <c r="L20" s="10">
         <v>4</v>
       </c>
       <c r="M20" s="1"/>
@@ -1238,14 +1486,14 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="C21" s="4">
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1259,16 +1507,16 @@
       <c r="H21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="7">
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="9" t="n">
+      <c r="K21" s="9">
         <v>90</v>
       </c>
-      <c r="L21" s="10" t="n">
+      <c r="L21" s="10">
         <v>4</v>
       </c>
       <c r="M21" s="1"/>
@@ -1286,14 +1534,14 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="4" t="n">
+      <c r="C22" s="4">
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1307,16 +1555,16 @@
       <c r="H22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="7" t="n">
+      <c r="I22" s="7">
         <v>30</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="9" t="n">
+      <c r="K22" s="9">
         <v>-1</v>
       </c>
-      <c r="L22" s="9" t="n">
+      <c r="L22" s="9">
         <v>3</v>
       </c>
       <c r="M22" s="1"/>
@@ -1334,14 +1582,14 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="10">
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -1355,16 +1603,16 @@
       <c r="H23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I23" s="7">
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="9" t="n">
+      <c r="K23" s="9">
         <v>-1</v>
       </c>
-      <c r="L23" s="9" t="n">
+      <c r="L23" s="9">
         <v>3</v>
       </c>
       <c r="M23" s="1"/>
@@ -1382,14 +1630,14 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="10">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1403,16 +1651,16 @@
       <c r="H24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="7" t="n">
+      <c r="I24" s="7">
         <v>30</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L24" s="9" t="n">
+      <c r="K24" s="9">
+        <v>15</v>
+      </c>
+      <c r="L24" s="9">
         <v>3</v>
       </c>
       <c r="M24" s="1"/>
@@ -1430,14 +1678,14 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="4">
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1451,16 +1699,16 @@
       <c r="H25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="7">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L25" s="9" t="n">
+      <c r="K25" s="9">
+        <v>15</v>
+      </c>
+      <c r="L25" s="9">
         <v>3</v>
       </c>
       <c r="M25" s="1"/>
@@ -1478,14 +1726,14 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="4" t="n">
+      <c r="C26" s="4">
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -1499,16 +1747,16 @@
       <c r="H26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I26" s="7">
         <v>30</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="9" t="n">
+      <c r="K26" s="9">
         <v>20</v>
       </c>
-      <c r="L26" s="9" t="n">
+      <c r="L26" s="9">
         <v>3</v>
       </c>
       <c r="M26" s="1"/>
@@ -1526,14 +1774,14 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="10">
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -1547,16 +1795,16 @@
       <c r="H27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="7">
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="9" t="n">
+      <c r="K27" s="9">
         <v>20</v>
       </c>
-      <c r="L27" s="9" t="n">
+      <c r="L27" s="9">
         <v>3</v>
       </c>
       <c r="M27" s="1"/>
@@ -1574,14 +1822,14 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="10">
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1595,16 +1843,16 @@
       <c r="H28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I28" s="7">
         <v>30</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L28" s="9" t="n">
+      <c r="K28" s="7">
+        <v>30</v>
+      </c>
+      <c r="L28" s="9">
         <v>3</v>
       </c>
       <c r="M28" s="1"/>
@@ -1622,14 +1870,14 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="4" t="n">
+      <c r="C29" s="4">
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -1643,16 +1891,16 @@
       <c r="H29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="7">
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L29" s="9" t="n">
+      <c r="K29" s="7">
+        <v>30</v>
+      </c>
+      <c r="L29" s="9">
         <v>3</v>
       </c>
       <c r="M29" s="1"/>
@@ -1670,14 +1918,14 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="4" t="n">
+      <c r="C30" s="4">
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -1691,16 +1939,16 @@
       <c r="H30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="7" t="n">
+      <c r="I30" s="7">
         <v>30</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="9" t="n">
+      <c r="K30" s="9">
         <v>90</v>
       </c>
-      <c r="L30" s="10" t="n">
+      <c r="L30" s="10">
         <v>3</v>
       </c>
       <c r="M30" s="1"/>
@@ -1718,14 +1966,14 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="10" t="n">
+      <c r="C31" s="10">
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -1739,16 +1987,16 @@
       <c r="H31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="7">
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="9" t="n">
+      <c r="K31" s="9">
         <v>90</v>
       </c>
-      <c r="L31" s="10" t="n">
+      <c r="L31" s="10">
         <v>3</v>
       </c>
       <c r="M31" s="1"/>
@@ -1766,14 +2014,14 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="10" t="n">
+      <c r="C32" s="10">
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1787,16 +2035,16 @@
       <c r="H32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="7" t="n">
+      <c r="I32" s="7">
         <v>30</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="9" t="n">
+      <c r="K32" s="9">
         <v>-1</v>
       </c>
-      <c r="L32" s="9" t="n">
+      <c r="L32" s="9">
         <v>4</v>
       </c>
       <c r="M32" s="1"/>
@@ -1814,14 +2062,14 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="4">
         <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1835,16 +2083,16 @@
       <c r="H33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="7" t="n">
+      <c r="I33" s="7">
         <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="9" t="n">
+      <c r="K33" s="9">
         <v>-1</v>
       </c>
-      <c r="L33" s="9" t="n">
+      <c r="L33" s="9">
         <v>4</v>
       </c>
       <c r="M33" s="1"/>
@@ -1862,14 +2110,14 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="4">
         <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -1883,16 +2131,16 @@
       <c r="H34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="7" t="n">
+      <c r="I34" s="7">
         <v>30</v>
       </c>
       <c r="J34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L34" s="9" t="n">
+      <c r="K34" s="9">
+        <v>15</v>
+      </c>
+      <c r="L34" s="9">
         <v>4</v>
       </c>
       <c r="M34" s="1"/>
@@ -1910,14 +2158,14 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="10" t="n">
+      <c r="C35" s="10">
         <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -1931,16 +2179,16 @@
       <c r="H35" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="7" t="n">
+      <c r="I35" s="7">
         <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L35" s="9" t="n">
+      <c r="K35" s="9">
+        <v>15</v>
+      </c>
+      <c r="L35" s="9">
         <v>4</v>
       </c>
       <c r="M35" s="1"/>
@@ -1958,14 +2206,14 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="10" t="n">
+      <c r="C36" s="10">
         <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -1979,16 +2227,16 @@
       <c r="H36" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="7" t="n">
+      <c r="I36" s="7">
         <v>30</v>
       </c>
       <c r="J36" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K36" s="9" t="n">
+      <c r="K36" s="9">
         <v>20</v>
       </c>
-      <c r="L36" s="9" t="n">
+      <c r="L36" s="9">
         <v>4</v>
       </c>
       <c r="M36" s="1"/>
@@ -2006,14 +2254,14 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="4" t="n">
+      <c r="C37" s="4">
         <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -2027,16 +2275,16 @@
       <c r="H37" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="7" t="n">
+      <c r="I37" s="7">
         <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K37" s="9" t="n">
+      <c r="K37" s="9">
         <v>20</v>
       </c>
-      <c r="L37" s="9" t="n">
+      <c r="L37" s="9">
         <v>4</v>
       </c>
       <c r="M37" s="1"/>
@@ -2054,14 +2302,14 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="4" t="n">
+      <c r="C38" s="4">
         <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -2075,16 +2323,16 @@
       <c r="H38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="7" t="n">
+      <c r="I38" s="7">
         <v>30</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L38" s="9" t="n">
+      <c r="K38" s="7">
+        <v>30</v>
+      </c>
+      <c r="L38" s="9">
         <v>4</v>
       </c>
       <c r="M38" s="1"/>
@@ -2102,14 +2350,14 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="10" t="n">
+      <c r="C39" s="10">
         <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -2123,16 +2371,16 @@
       <c r="H39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="7" t="n">
+      <c r="I39" s="7">
         <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K39" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L39" s="9" t="n">
+      <c r="K39" s="7">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
         <v>4</v>
       </c>
       <c r="M39" s="1"/>
@@ -2150,14 +2398,14 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="10" t="n">
+      <c r="C40" s="10">
         <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -2171,16 +2419,16 @@
       <c r="H40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="7" t="n">
+      <c r="I40" s="7">
         <v>30</v>
       </c>
       <c r="J40" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="9" t="n">
+      <c r="K40" s="9">
         <v>90</v>
       </c>
-      <c r="L40" s="10" t="n">
+      <c r="L40" s="10">
         <v>4</v>
       </c>
       <c r="M40" s="1"/>
@@ -2198,14 +2446,14 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="4" t="n">
+      <c r="C41" s="4">
         <v>40</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -2219,16 +2467,16 @@
       <c r="H41" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="7" t="n">
+      <c r="I41" s="7">
         <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K41" s="9" t="n">
+      <c r="K41" s="9">
         <v>90</v>
       </c>
-      <c r="L41" s="10" t="n">
+      <c r="L41" s="10">
         <v>4</v>
       </c>
       <c r="M41" s="1"/>
@@ -2247,12 +2495,7 @@
       <c r="Z41" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified errors with Cst6 TF group reps 2&3 (incorrect fastq files and reads) and then deleted the failed libraries of Rep 3 that did not have spike in or full run
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.07.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB13F63-B3D2-5F44-A4E6-8AF98252FA9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E27F36-8049-6C4E-B779-D97BA96C11C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="13200" windowHeight="19840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="20">
   <si>
     <t>harvestDate</t>
   </si>
@@ -143,7 +143,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -516,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z41"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -527,11 +527,11 @@
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="7" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" customWidth="1"/>
@@ -646,7 +646,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="18">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>14</v>
@@ -662,14 +662,14 @@
       <c r="I3" s="15">
         <v>30</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>18</v>
+      <c r="J3" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K3" s="17">
         <v>-1</v>
       </c>
       <c r="L3" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
@@ -693,8 +693,8 @@
       <c r="B4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="18">
-        <v>3</v>
+      <c r="C4" s="12">
+        <v>12</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>14</v>
@@ -710,14 +710,14 @@
       <c r="I4" s="15">
         <v>30</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>17</v>
+      <c r="J4" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="K4" s="17">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="L4" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
@@ -742,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="12">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>14</v>
@@ -758,14 +758,14 @@
       <c r="I5" s="15">
         <v>30</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>18</v>
+      <c r="J5" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K5" s="17">
         <v>15</v>
       </c>
       <c r="L5" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -789,8 +789,8 @@
       <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="12">
-        <v>5</v>
+      <c r="C6" s="18">
+        <v>14</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>14</v>
@@ -806,14 +806,14 @@
       <c r="I6" s="15">
         <v>30</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>17</v>
+      <c r="J6" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="K6" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L6" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -838,7 +838,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="18">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>14</v>
@@ -854,14 +854,14 @@
       <c r="I7" s="15">
         <v>30</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>18</v>
+      <c r="J7" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K7" s="17">
         <v>20</v>
       </c>
       <c r="L7" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -885,8 +885,8 @@
       <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="18">
-        <v>7</v>
+      <c r="C8" s="12">
+        <v>16</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>14</v>
@@ -902,14 +902,14 @@
       <c r="I8" s="15">
         <v>30</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="15">
-        <v>30</v>
+      <c r="J8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="17">
+        <v>20</v>
       </c>
       <c r="L8" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -934,7 +934,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="12">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>14</v>
@@ -950,14 +950,14 @@
       <c r="I9" s="15">
         <v>30</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>18</v>
+      <c r="J9" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K9" s="15">
         <v>30</v>
       </c>
       <c r="L9" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -981,8 +981,8 @@
       <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12">
-        <v>9</v>
+      <c r="C10" s="18">
+        <v>18</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>14</v>
@@ -998,14 +998,14 @@
       <c r="I10" s="15">
         <v>30</v>
       </c>
-      <c r="J10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="17">
-        <v>90</v>
-      </c>
-      <c r="L10" s="18">
-        <v>3</v>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="15">
+        <v>30</v>
+      </c>
+      <c r="L10" s="17">
+        <v>4</v>
       </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -1030,7 +1030,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="18">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>14</v>
@@ -1046,14 +1046,14 @@
       <c r="I11" s="15">
         <v>30</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>18</v>
+      <c r="J11" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K11" s="17">
         <v>90</v>
       </c>
       <c r="L11" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -1077,8 +1077,8 @@
       <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="18">
-        <v>11</v>
+      <c r="C12" s="12">
+        <v>20</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>14</v>
@@ -1094,13 +1094,13 @@
       <c r="I12" s="15">
         <v>30</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>17</v>
+      <c r="J12" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="K12" s="17">
-        <v>-1</v>
-      </c>
-      <c r="L12" s="17">
+        <v>90</v>
+      </c>
+      <c r="L12" s="18">
         <v>4</v>
       </c>
       <c r="M12" s="9"/>
@@ -1125,8 +1125,8 @@
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="12">
-        <v>12</v>
+      <c r="C13" s="18">
+        <v>31</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>14</v>
@@ -1134,7 +1134,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>16</v>
@@ -1142,8 +1142,8 @@
       <c r="I13" s="15">
         <v>30</v>
       </c>
-      <c r="J13" s="9" t="s">
-        <v>18</v>
+      <c r="J13" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K13" s="17">
         <v>-1</v>
@@ -1174,7 +1174,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="12">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>14</v>
@@ -1182,7 +1182,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>16</v>
@@ -1190,11 +1190,11 @@
       <c r="I14" s="15">
         <v>30</v>
       </c>
-      <c r="J14" s="16" t="s">
-        <v>17</v>
+      <c r="J14" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="K14" s="17">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="L14" s="17">
         <v>4</v>
@@ -1221,8 +1221,8 @@
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="18">
-        <v>14</v>
+      <c r="C15" s="12">
+        <v>33</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>14</v>
@@ -1230,7 +1230,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>16</v>
@@ -1238,8 +1238,8 @@
       <c r="I15" s="15">
         <v>30</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>18</v>
+      <c r="J15" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K15" s="17">
         <v>15</v>
@@ -1270,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="18">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>14</v>
@@ -1278,19 +1278,19 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="15">
+        <v>30</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="17">
         <v>15</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="15">
-        <v>30</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="17">
-        <v>20</v>
       </c>
       <c r="L16" s="17">
         <v>4</v>
@@ -1317,8 +1317,8 @@
       <c r="B17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="12">
-        <v>16</v>
+      <c r="C17" s="18">
+        <v>35</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>14</v>
@@ -1326,7 +1326,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>16</v>
@@ -1334,8 +1334,8 @@
       <c r="I17" s="15">
         <v>30</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>18</v>
+      <c r="J17" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K17" s="17">
         <v>20</v>
@@ -1366,7 +1366,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="12">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>14</v>
@@ -1374,7 +1374,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>16</v>
@@ -1382,11 +1382,11 @@
       <c r="I18" s="15">
         <v>30</v>
       </c>
-      <c r="J18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="15">
-        <v>30</v>
+      <c r="J18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="17">
+        <v>20</v>
       </c>
       <c r="L18" s="17">
         <v>4</v>
@@ -1413,8 +1413,8 @@
       <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="18">
-        <v>18</v>
+      <c r="C19" s="12">
+        <v>37</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>14</v>
@@ -1422,7 +1422,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>16</v>
@@ -1430,8 +1430,8 @@
       <c r="I19" s="15">
         <v>30</v>
       </c>
-      <c r="J19" s="9" t="s">
-        <v>18</v>
+      <c r="J19" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K19" s="15">
         <v>30</v>
@@ -1462,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="18">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>14</v>
@@ -1470,7 +1470,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>16</v>
@@ -1478,13 +1478,13 @@
       <c r="I20" s="15">
         <v>30</v>
       </c>
-      <c r="J20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="17">
-        <v>90</v>
-      </c>
-      <c r="L20" s="18">
+      <c r="J20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="15">
+        <v>30</v>
+      </c>
+      <c r="L20" s="17">
         <v>4</v>
       </c>
       <c r="M20" s="9"/>
@@ -1509,8 +1509,8 @@
       <c r="B21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="12">
-        <v>20</v>
+      <c r="C21" s="18">
+        <v>39</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>14</v>
@@ -1518,7 +1518,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H21" s="14" t="s">
         <v>16</v>
@@ -1526,8 +1526,8 @@
       <c r="I21" s="15">
         <v>30</v>
       </c>
-      <c r="J21" s="9" t="s">
-        <v>18</v>
+      <c r="J21" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K21" s="17">
         <v>90</v>
@@ -1551,40 +1551,40 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="12">
-        <v>21</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="14" t="s">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="15">
-        <v>30</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="17">
-        <v>-1</v>
-      </c>
-      <c r="L22" s="17">
-        <v>3</v>
-      </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
+      <c r="H22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="6">
+        <v>30</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="7">
+        <v>90</v>
+      </c>
+      <c r="L22" s="8">
+        <v>4</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -1598,918 +1598,6 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="18">
-        <v>22</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="15">
-        <v>30</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="17">
-        <v>-1</v>
-      </c>
-      <c r="L23" s="17">
-        <v>3</v>
-      </c>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-    </row>
-    <row r="24" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="18">
-        <v>23</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="15">
-        <v>30</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="17">
-        <v>15</v>
-      </c>
-      <c r="L24" s="17">
-        <v>3</v>
-      </c>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-    </row>
-    <row r="25" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="12">
-        <v>24</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="15">
-        <v>30</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K25" s="17">
-        <v>15</v>
-      </c>
-      <c r="L25" s="17">
-        <v>3</v>
-      </c>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-    </row>
-    <row r="26" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="12">
-        <v>25</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="15">
-        <v>30</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="17">
-        <v>20</v>
-      </c>
-      <c r="L26" s="17">
-        <v>3</v>
-      </c>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-    </row>
-    <row r="27" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="18">
-        <v>26</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="15">
-        <v>30</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="17">
-        <v>20</v>
-      </c>
-      <c r="L27" s="17">
-        <v>3</v>
-      </c>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-    </row>
-    <row r="28" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="18">
-        <v>27</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="15">
-        <v>30</v>
-      </c>
-      <c r="J28" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="15">
-        <v>30</v>
-      </c>
-      <c r="L28" s="17">
-        <v>3</v>
-      </c>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-    </row>
-    <row r="29" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="12">
-        <v>28</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="15">
-        <v>30</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="15">
-        <v>30</v>
-      </c>
-      <c r="L29" s="17">
-        <v>3</v>
-      </c>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-    </row>
-    <row r="30" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="12">
-        <v>29</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="15">
-        <v>30</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="17">
-        <v>90</v>
-      </c>
-      <c r="L30" s="18">
-        <v>3</v>
-      </c>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="18">
-        <v>30</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="15">
-        <v>30</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="17">
-        <v>90</v>
-      </c>
-      <c r="L31" s="18">
-        <v>3</v>
-      </c>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-    </row>
-    <row r="32" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="18">
-        <v>31</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="15">
-        <v>30</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="17">
-        <v>-1</v>
-      </c>
-      <c r="L32" s="17">
-        <v>4</v>
-      </c>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-    </row>
-    <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="12">
-        <v>32</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="15">
-        <v>30</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" s="17">
-        <v>-1</v>
-      </c>
-      <c r="L33" s="17">
-        <v>4</v>
-      </c>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-    </row>
-    <row r="34" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="12">
-        <v>33</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="15">
-        <v>30</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="17">
-        <v>15</v>
-      </c>
-      <c r="L34" s="17">
-        <v>4</v>
-      </c>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-    </row>
-    <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="18">
-        <v>34</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="15">
-        <v>30</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="17">
-        <v>15</v>
-      </c>
-      <c r="L35" s="17">
-        <v>4</v>
-      </c>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
-      <c r="Z35" s="1"/>
-    </row>
-    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="18">
-        <v>35</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="15">
-        <v>30</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="17">
-        <v>20</v>
-      </c>
-      <c r="L36" s="17">
-        <v>4</v>
-      </c>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
-      <c r="Z36" s="1"/>
-    </row>
-    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="12">
-        <v>36</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="15">
-        <v>30</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="17">
-        <v>20</v>
-      </c>
-      <c r="L37" s="17">
-        <v>4</v>
-      </c>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-    </row>
-    <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="12">
-        <v>37</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="15">
-        <v>30</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="15">
-        <v>30</v>
-      </c>
-      <c r="L38" s="17">
-        <v>4</v>
-      </c>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-    </row>
-    <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="18">
-        <v>38</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="15">
-        <v>30</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="15">
-        <v>30</v>
-      </c>
-      <c r="L39" s="17">
-        <v>4</v>
-      </c>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-    </row>
-    <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="18">
-        <v>39</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="15">
-        <v>30</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="17">
-        <v>90</v>
-      </c>
-      <c r="L40" s="18">
-        <v>4</v>
-      </c>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-      <c r="Y40" s="1"/>
-      <c r="Z40" s="1"/>
-    </row>
-    <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="3">
-        <v>40</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="6">
-        <v>30</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K41" s="7">
-        <v>90</v>
-      </c>
-      <c r="L41" s="8">
-        <v>4</v>
-      </c>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
-      <c r="X41" s="1"/>
-      <c r="Y41" s="1"/>
-      <c r="Z41" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>